<commit_message>
Mise au point du service Dark Sky qui s'avère bien foutu: - Conversion de la vitesse du vent en km/h en système métrique. - Mise au point des css des conditions. - PHPDoc sur le fichier du service.
git-svn-id: svn://zone.spip.org/spip-zone/_plugins_@122806 ac52e18a-acf5-0310-9fe8-c4428f23b10a
</commit_message>
<xml_diff>
--- a/rainette/trunk/services/codes.xlsx
+++ b/rainette/trunk/services/codes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Sites/SPIP/plugins/rainette/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C83AD2A-E49B-5B40-B2B8-824023E7E41B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="460" windowWidth="26940" windowHeight="22480" tabRatio="500"/>
+    <workbookView xWindow="-24100" yWindow="460" windowWidth="10000" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="Apixu_weather_conditions" localSheetId="0">Feuil1!$I$2:$N$50</definedName>
     <definedName name="Multilingual_Weather_Conditions" localSheetId="0">Feuil1!$P$2:$X$1002</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,8 +33,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Apixu_weather_conditions" type="6" refreshedVersion="0" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Apixu_weather_conditions" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/eric/Downloads/Apixu_weather_conditions.csv" decimal="," thousands=" " comma="1">
       <textFields count="4">
         <textField/>
@@ -43,7 +44,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="Multilingual_Weather_Conditions" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="Multilingual_Weather_Conditions" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/eric/Downloads/Multilingual_Weather_Conditions.csv" decimal="," thousands=" " comma="1">
       <textFields count="7">
         <textField/>
@@ -866,7 +867,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -991,16 +992,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Multilingual_Weather_Conditions" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Multilingual_Weather_Conditions" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Apixu_weather_conditions" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Apixu_weather_conditions" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1265,11 +1269,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X967"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1282,15 +1286,15 @@
     <col min="6" max="6" width="31.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="10.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="4.83203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="5.83203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="40.33203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="5" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="5.1640625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="6" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="44.83203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="41.1640625" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="47.33203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="5.83203125" style="3" customWidth="1"/>
+    <col min="9" max="11" width="5.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="40.33203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="5" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="5.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="6" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="44.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="41.1640625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="47.33203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="5.83203125" style="3" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26.5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="3.5" style="3" customWidth="1"/>
@@ -3774,7 +3778,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="P3:S50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P3:S50">
     <sortCondition ref="P3:P50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3783,7 +3787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A47"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">

</xml_diff>